<commit_message>
Building website with new test case examples
</commit_message>
<xml_diff>
--- a/ValueSet-CBSCDCAddressUseVS.xlsx
+++ b/ValueSet-CBSCDCAddressUseVS.xlsx
@@ -7,7 +7,7 @@
   </bookViews>
   <sheets>
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
-    <sheet name="Include from Case Based Surveil" r:id="rId4" sheetId="2"/>
+    <sheet name="Include from Case Based Surve" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2021-10-18T11:18:26-04:00</t>
+    <t>2021-11-01T11:33:34-04:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Update to GH Pages
</commit_message>
<xml_diff>
--- a/ValueSet-CBSCDCAddressUseVS.xlsx
+++ b/ValueSet-CBSCDCAddressUseVS.xlsx
@@ -7,7 +7,7 @@
   </bookViews>
   <sheets>
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
-    <sheet name="Include from Case Based Surve" r:id="rId4" sheetId="2"/>
+    <sheet name="Include from Case Based Surveil" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2021-11-01T11:33:34-04:00</t>
+    <t>2021-11-03T10:06:32-04:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>